<commit_message>
Update ACMO sample file
</commit_message>
<xml_diff>
--- a/Temlpates/ACMO/ACMO_templates.xlsx
+++ b/Temlpates/ACMO/ACMO_templates.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="386">
   <si>
     <t>decimal degrees</t>
   </si>
@@ -2399,7 +2399,7 @@
       <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2633,8 +2633,12 @@
       <c r="D2" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="E2" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>180</v>
+      </c>
       <c r="G2" s="24" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Update ACMO template to version 4.1.0
Add new model output variable as follow
EPCM- Total season transpiration (mm)
ESCM- Total season soil evaporation (mm)
</commit_message>
<xml_diff>
--- a/Temlpates/ACMO/ACMO_templates.xlsx
+++ b/Temlpates/ACMO/ACMO_templates.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="168" windowWidth="13392" windowHeight="5076"/>
   </bookViews>
   <sheets>
-    <sheet name="ACMO_ver4.0.1" sheetId="3" r:id="rId1"/>
+    <sheet name="ACMO_ver4.1.0" sheetId="3" r:id="rId1"/>
     <sheet name="ClimateScenarioCodes" sheetId="6" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="390">
   <si>
     <t>decimal degrees</t>
   </si>
@@ -1242,6 +1242,18 @@
   </si>
   <si>
     <t>Unique hash assigned when rotational analysis DOME files are loaded into ACE database</t>
+  </si>
+  <si>
+    <t>EPCM_S</t>
+  </si>
+  <si>
+    <t>ESCM_S</t>
+  </si>
+  <si>
+    <t>Total season transpiration</t>
+  </si>
+  <si>
+    <t>Total season soil evaporation</t>
   </si>
 </sst>
 </file>
@@ -2393,13 +2405,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BE82"/>
+  <dimension ref="A1:BF82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2452,7 +2464,7 @@
     <col min="57" max="57" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="22" customFormat="1" ht="177.75" customHeight="1">
+    <row r="1" spans="1:58" s="22" customFormat="1" ht="177.75" customHeight="1">
       <c r="A1" s="24" t="s">
         <v>213</v>
       </c>
@@ -2619,8 +2631,14 @@
       <c r="BD1" s="23" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="2" spans="1:57" s="22" customFormat="1" ht="28.8">
+      <c r="BE1" s="23" t="s">
+        <v>388</v>
+      </c>
+      <c r="BF1" s="23" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" s="22" customFormat="1" ht="28.8">
       <c r="A2" s="24" t="s">
         <v>213</v>
       </c>
@@ -2789,8 +2807,14 @@
       <c r="BD2" s="23" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:57" s="21" customFormat="1">
+      <c r="BE2" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="BF2" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" s="21" customFormat="1">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -2959,8 +2983,14 @@
       <c r="BD3" s="31" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="4" spans="1:57">
+      <c r="BE3" s="31" t="s">
+        <v>386</v>
+      </c>
+      <c r="BF3" s="31" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58">
       <c r="A4" s="17" t="s">
         <v>187</v>
       </c>
@@ -3096,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:57">
+    <row r="5" spans="1:58">
       <c r="A5" s="17" t="s">
         <v>187</v>
       </c>
@@ -3230,7 +3260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:57">
+    <row r="6" spans="1:58">
       <c r="A6" s="17" t="s">
         <v>187</v>
       </c>
@@ -3362,7 +3392,7 @@
       </c>
       <c r="BE6" s="16"/>
     </row>
-    <row r="7" spans="1:57">
+    <row r="7" spans="1:58">
       <c r="A7" s="17" t="s">
         <v>187</v>
       </c>
@@ -3497,7 +3527,7 @@
       </c>
       <c r="BE7" s="4"/>
     </row>
-    <row r="8" spans="1:57">
+    <row r="8" spans="1:58">
       <c r="A8" s="17" t="s">
         <v>187</v>
       </c>
@@ -3628,7 +3658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:57">
+    <row r="9" spans="1:58">
       <c r="A9" s="17" t="s">
         <v>187</v>
       </c>
@@ -3759,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:57">
+    <row r="10" spans="1:58">
       <c r="A10" s="17" t="s">
         <v>187</v>
       </c>
@@ -3890,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:57">
+    <row r="11" spans="1:58">
       <c r="A11" s="17" t="s">
         <v>187</v>
       </c>
@@ -4021,7 +4051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:57">
+    <row r="12" spans="1:58">
       <c r="A12" s="17" t="s">
         <v>187</v>
       </c>
@@ -4152,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:57">
+    <row r="13" spans="1:58">
       <c r="A13" s="17" t="s">
         <v>187</v>
       </c>
@@ -4286,7 +4316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:57">
+    <row r="14" spans="1:58">
       <c r="A14" s="17" t="s">
         <v>187</v>
       </c>
@@ -4420,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:57">
+    <row r="15" spans="1:58">
       <c r="A15" s="17" t="s">
         <v>187</v>
       </c>
@@ -4554,7 +4584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:57">
+    <row r="16" spans="1:58">
       <c r="A16" s="17" t="s">
         <v>187</v>
       </c>
@@ -9945,7 +9975,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
@@ -10651,16 +10683,32 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="13.8" thickBot="1">
-      <c r="A57" s="34"/>
-      <c r="B57" s="33"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="33"/>
+      <c r="A57" s="55" t="s">
+        <v>386</v>
+      </c>
+      <c r="B57" s="55" t="s">
+        <v>388</v>
+      </c>
+      <c r="C57" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="13.8" thickBot="1">
-      <c r="A58" s="34"/>
-      <c r="B58" s="33"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="33"/>
+      <c r="A58" s="55" t="s">
+        <v>387</v>
+      </c>
+      <c r="B58" s="55" t="s">
+        <v>389</v>
+      </c>
+      <c r="C58" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="13.8" thickBot="1">
       <c r="A59" s="34"/>

</xml_diff>